<commit_message>
Supply Chain: Add network optimization
</commit_message>
<xml_diff>
--- a/apps/supply_chain/InputDataProductionSolver.xlsx
+++ b/apps/supply_chain/InputDataProductionSolver.xlsx
@@ -5,17 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
-    <sheet name="Demand" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="StartingInventory" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Rate" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="AvailableCapacity" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="TransportationCosts" sheetId="5" state="visible" r:id="rId6"/>
-    <sheet name="TransferLanes" sheetId="6" state="visible" r:id="rId7"/>
-    <sheet name="TargetStocks" sheetId="7" state="visible" r:id="rId8"/>
-    <sheet name="LocationCapacity" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="DemandByLocation" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="DemandByCustomer" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="ShipmentLanes" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="StartingInventory" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Rate" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="AvailableCapacity" sheetId="6" state="visible" r:id="rId7"/>
+    <sheet name="TransportationCosts" sheetId="7" state="visible" r:id="rId8"/>
+    <sheet name="TransferLanes" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="TargetStocks" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="LocationCapacity" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="404" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="501" uniqueCount="47">
   <si>
     <t xml:space="preserve">Product</t>
   </si>
@@ -92,6 +94,30 @@
     <t xml:space="preserve">12 constraints in reality</t>
   </si>
   <si>
+    <t xml:space="preserve">Customer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supermarket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restaurant</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bulk</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bakery 1</t>
+  </si>
+  <si>
     <t xml:space="preserve">Resource</t>
   </si>
   <si>
@@ -119,9 +145,6 @@
     <t xml:space="preserve">TotalCapacityPerPeriod</t>
   </si>
   <si>
-    <t xml:space="preserve">Unit</t>
-  </si>
-  <si>
     <t xml:space="preserve">Oven</t>
   </si>
   <si>
@@ -138,9 +161,6 @@
   </si>
   <si>
     <t xml:space="preserve">Allowed?</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cost</t>
   </si>
   <si>
     <t xml:space="preserve">YES</t>
@@ -192,12 +212,18 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -234,7 +260,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -248,6 +274,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -282,7 +316,7 @@
       <selection pane="topLeft" activeCell="Q26" activeCellId="0" sqref="Q26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.83"/>
@@ -2572,7 +2606,728 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:E47"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>45323</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="4" t="n">
+        <v>45323</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="4" t="n">
+        <v>45323</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>45323</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>45323</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="4"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="4" t="n">
+        <v>45292</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="4" t="n">
+        <v>45323</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="4" t="n">
+        <v>45352</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="4" t="n">
+        <v>45383</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="4" t="n">
+        <v>45413</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="4" t="n">
+        <v>45444</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D16" s="5"/>
+    </row>
+    <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C17" s="4" t="n">
+        <v>45292</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C18" s="4" t="n">
+        <v>45292</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="4" t="n">
+        <v>45292</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="4" t="n">
+        <v>45352</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="4" t="n">
+        <v>45352</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="4" t="n">
+        <v>45352</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C27" s="4" t="n">
+        <v>45383</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="4" t="n">
+        <v>45383</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C29" s="4" t="n">
+        <v>45383</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C31" s="4" t="n">
+        <v>45413</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C32" s="4" t="n">
+        <v>45413</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C33" s="4" t="n">
+        <v>45413</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C34" s="4" t="n">
+        <v>45413</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C35" s="4" t="n">
+        <v>45413</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C37" s="4" t="n">
+        <v>45383</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C38" s="4" t="n">
+        <v>45383</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C39" s="4" t="n">
+        <v>45383</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C40" s="4" t="n">
+        <v>45383</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C41" s="4" t="n">
+        <v>45383</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C43" s="4" t="n">
+        <v>45444</v>
+      </c>
+      <c r="D43" s="0" t="n">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C44" s="4" t="n">
+        <v>45444</v>
+      </c>
+      <c r="D44" s="0" t="n">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C45" s="4" t="n">
+        <v>45444</v>
+      </c>
+      <c r="D45" s="0" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C46" s="4" t="n">
+        <v>45444</v>
+      </c>
+      <c r="D46" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C47" s="4" t="n">
+        <v>45444</v>
+      </c>
+      <c r="D47" s="0" t="n">
+        <v>105</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:D11"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -2583,7 +3338,7 @@
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8.67"/>
   </cols>
@@ -3766,7 +4521,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
@@ -3777,23 +4532,23 @@
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3801,16 +4556,16 @@
         <v>15</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C2" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="C2" s="6" t="n">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3818,16 +4573,16 @@
         <v>15</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="C3" s="6" t="n">
         <v>3</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3835,16 +4590,16 @@
         <v>11</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="C4" s="4" t="n">
+        <v>35</v>
+      </c>
+      <c r="C4" s="6" t="n">
         <v>2</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3852,16 +4607,16 @@
         <v>11</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="4" t="n">
+        <v>32</v>
+      </c>
+      <c r="C5" s="6" t="n">
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3869,16 +4624,16 @@
         <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="C6" s="6" t="n">
         <v>5</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3886,16 +4641,16 @@
         <v>11</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C7" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="C7" s="6" t="n">
         <v>4</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3903,16 +4658,16 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C8" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="C8" s="6" t="n">
         <v>6</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3920,16 +4675,16 @@
         <v>14</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="C9" s="4" t="n">
+        <v>36</v>
+      </c>
+      <c r="C9" s="6" t="n">
         <v>5</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3937,16 +4692,16 @@
         <v>14</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C10" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="C10" s="6" t="n">
         <v>7</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -3954,357 +4709,17 @@
         <v>13</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C11" s="4" t="n">
+        <v>34</v>
+      </c>
+      <c r="C11" s="6" t="n">
         <v>10</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D1048576"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.16"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C2" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
         <v>33</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>12</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B5" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>8</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:D31"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="14.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C2" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D2" s="4" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="D4" s="4" t="n">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="4"/>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="4"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="4"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="4"/>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="4"/>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="4"/>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="4"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="4"/>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="4"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="5"/>
-      <c r="D15" s="4"/>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="4"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="4"/>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="4"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="5"/>
-      <c r="D19" s="4"/>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="4"/>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="4"/>
-    </row>
-    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="4"/>
-    </row>
-    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="4"/>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="4"/>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="5"/>
-      <c r="D25" s="4"/>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="4"/>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="5"/>
-      <c r="D27" s="4"/>
-    </row>
-    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="4"/>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="5"/>
-      <c r="D29" s="4"/>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="4"/>
-    </row>
-    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="5"/>
-      <c r="D31" s="4"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4322,113 +4737,88 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.16"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>29</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>34</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>35</v>
+        <v>37</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B3" s="1" t="s">
+      <c r="A3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>10</v>
+      <c r="C3" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
+      <c r="A4" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
@@ -4445,101 +4835,231 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>41</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>39</v>
+        <v>43</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D2" s="6" t="n">
+        <v>5</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="0" t="n">
-        <v>20</v>
+      <c r="C3" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D3" s="6" t="n">
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="0" t="n">
-        <v>40</v>
+        <v>12</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="6" t="n">
+        <v>15</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="0" t="n">
-        <v>25</v>
-      </c>
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="0" t="n">
-        <v>30</v>
-      </c>
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>30</v>
-      </c>
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="7"/>
+      <c r="D8" s="6"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="C9" s="0" t="n">
-        <v>15</v>
-      </c>
+      <c r="A9" s="1"/>
+      <c r="B9" s="1"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="6"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C10" s="0" t="n">
-        <v>20</v>
-      </c>
+      <c r="A10" s="1"/>
+      <c r="B10" s="1"/>
+      <c r="C10" s="7"/>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1"/>
+      <c r="B11" s="1"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1"/>
+      <c r="B12" s="1"/>
+      <c r="C12" s="7"/>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="1"/>
+      <c r="B13" s="1"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="7"/>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="1"/>
+      <c r="B21" s="1"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="1"/>
+      <c r="B22" s="1"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="6"/>
+    </row>
+    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="7"/>
+      <c r="D24" s="6"/>
+    </row>
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="6"/>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="7"/>
+      <c r="D26" s="6"/>
+    </row>
+    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="6"/>
+    </row>
+    <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="7"/>
+      <c r="D28" s="6"/>
+    </row>
+    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="6"/>
+    </row>
+    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="7"/>
+      <c r="D30" s="6"/>
+    </row>
+    <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="6"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4557,44 +5077,223 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5234375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="0" t="n">
-        <v>100</v>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="0" t="n">
-        <v>100</v>
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:C10"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>40</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" s="0" t="n">
-        <v>200</v>
+        <v>6</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Supply Chain: use same data for both problem types
</commit_message>
<xml_diff>
--- a/apps/supply_chain/InputDataProductionSolver.xlsx
+++ b/apps/supply_chain/InputDataProductionSolver.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="DemandByLocation" sheetId="1" state="visible" r:id="rId2"/>
@@ -316,7 +316,7 @@
       <selection pane="topLeft" activeCell="Q26" activeCellId="0" sqref="Q26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="12.83"/>
@@ -2614,10 +2614,10 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -2648,7 +2648,7 @@
         <v>10</v>
       </c>
       <c r="B5" s="0" t="n">
-        <v>200</v>
+        <v>100</v>
       </c>
     </row>
   </sheetData>
@@ -2673,7 +2673,7 @@
       <selection pane="topLeft" activeCell="E9" activeCellId="0" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3208,11 +3208,11 @@
   </sheetPr>
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C14" activeCellId="0" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -3338,7 +3338,7 @@
       <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="1" style="0" width="8.67"/>
   </cols>
@@ -4532,7 +4532,7 @@
       <selection pane="topLeft" activeCell="C12" activeCellId="0" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -4739,11 +4739,11 @@
   </sheetPr>
   <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="19.16"/>
   </cols>
@@ -4770,7 +4770,7 @@
         <v>7</v>
       </c>
       <c r="C2" s="0" t="n">
-        <v>12</v>
+        <v>50</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>39</v>
@@ -4784,7 +4784,7 @@
         <v>7</v>
       </c>
       <c r="C3" s="0" t="n">
-        <v>12</v>
+        <v>40</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>39</v>
@@ -4798,7 +4798,7 @@
         <v>12</v>
       </c>
       <c r="C4" s="0" t="n">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>39</v>
@@ -4812,7 +4812,7 @@
         <v>12</v>
       </c>
       <c r="C5" s="0" t="n">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="D5" s="1" t="s">
         <v>39</v>
@@ -4841,7 +4841,7 @@
       <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="14.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5083,7 +5083,7 @@
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -5206,7 +5206,7 @@
       <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">

</xml_diff>